<commit_message>
Updated riverinfo.xlsx with haronr for all WGNAS rivers
</commit_message>
<xml_diff>
--- a/data-raw/riverinfo.xlsx
+++ b/data-raw/riverinfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NoBackup\rpkgs\DCFsers\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NoBackup\SLU-Aqua-salmonids\DCF\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
   <si>
     <t>haronr</t>
   </si>
   <si>
-    <t xml:space="preserve">Kalixälven  </t>
-  </si>
-  <si>
     <t>Råneälven</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Emån</t>
   </si>
   <si>
-    <t xml:space="preserve"> Mörrumsån</t>
-  </si>
-  <si>
     <t>haroname</t>
   </si>
   <si>
@@ -81,19 +75,190 @@
   </si>
   <si>
     <t>rivername</t>
+  </si>
+  <si>
+    <t>Alslövsån</t>
+  </si>
+  <si>
+    <t>Kalixälven</t>
+  </si>
+  <si>
+    <t>Bratteforsån</t>
+  </si>
+  <si>
+    <t>Bäveån</t>
+  </si>
+  <si>
+    <t>Fageredsån</t>
+  </si>
+  <si>
+    <t>Forsån</t>
+  </si>
+  <si>
+    <t>Grönån</t>
+  </si>
+  <si>
+    <t>Kungsbackaån</t>
+  </si>
+  <si>
+    <t>Munkedalsälven</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Pinnån</t>
+  </si>
+  <si>
+    <t>Sennan</t>
+  </si>
+  <si>
+    <t>Smedjeån</t>
+  </si>
+  <si>
+    <t>Storån</t>
+  </si>
+  <si>
+    <t>Strömsån</t>
+  </si>
+  <si>
+    <t>Surtan</t>
+  </si>
+  <si>
+    <t>Suseån</t>
+  </si>
+  <si>
+    <t>Säveån</t>
+  </si>
+  <si>
+    <t>Tvååkers kanal</t>
+  </si>
+  <si>
+    <t>Törlan</t>
+  </si>
+  <si>
+    <t>Vessingeån</t>
+  </si>
+  <si>
+    <t>Viskan</t>
+  </si>
+  <si>
+    <t>Örekilsälven</t>
+  </si>
+  <si>
+    <t>Arödsån</t>
+  </si>
+  <si>
+    <t>Brattorpsån</t>
+  </si>
+  <si>
+    <t>Brostorpsån</t>
+  </si>
+  <si>
+    <t>Edenbergaån</t>
+  </si>
+  <si>
+    <t>Enningdalsälven</t>
+  </si>
+  <si>
+    <t>Fylleån</t>
+  </si>
+  <si>
+    <t>Himleån</t>
+  </si>
+  <si>
+    <t>Hämmensån</t>
+  </si>
+  <si>
+    <t>Högvadsån</t>
+  </si>
+  <si>
+    <t>Lindomeån</t>
+  </si>
+  <si>
+    <t>Långevallsälven</t>
+  </si>
+  <si>
+    <t>Löftaån</t>
+  </si>
+  <si>
+    <t>Rolfsån</t>
+  </si>
+  <si>
+    <t>Rönneå</t>
+  </si>
+  <si>
+    <t>Rördalsån</t>
+  </si>
+  <si>
+    <t>Rössjöholmsån</t>
+  </si>
+  <si>
+    <t>Slissån</t>
+  </si>
+  <si>
+    <t>Sollumsån</t>
+  </si>
+  <si>
+    <t>Stensån</t>
+  </si>
+  <si>
+    <t>Sörån</t>
+  </si>
+  <si>
+    <t>Vättlandsån</t>
+  </si>
+  <si>
+    <t>Ätran</t>
+  </si>
+  <si>
+    <t>Bäljane å</t>
+  </si>
+  <si>
+    <t>Genevadsån</t>
+  </si>
+  <si>
+    <t>Göta älv</t>
+  </si>
+  <si>
+    <t>Rönne å</t>
+  </si>
+  <si>
+    <t>Lagan</t>
+  </si>
+  <si>
+    <t>Mellan Viskan och Rolfsån</t>
+  </si>
+  <si>
+    <t>Mellan Göta älv och Bäveån</t>
+  </si>
+  <si>
+    <t>Mellan Ätran och Himleån</t>
+  </si>
+  <si>
+    <t>Mörrumsån</t>
+  </si>
+  <si>
+    <t>Kynne älv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,8 +281,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,24 +564,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -423,10 +587,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1000</v>
@@ -434,10 +598,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>4000</v>
@@ -445,10 +609,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>7000</v>
@@ -456,10 +620,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>17000</v>
@@ -467,10 +631,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>18000</v>
@@ -478,10 +642,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>19000</v>
@@ -489,10 +653,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>24000</v>
@@ -500,10 +664,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>26000</v>
@@ -511,10 +675,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>28000</v>
@@ -522,10 +686,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>30000</v>
@@ -533,10 +697,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>32000</v>
@@ -544,10 +708,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>42000</v>
@@ -555,10 +719,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>51000</v>
@@ -566,10 +730,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>74000</v>
@@ -577,13 +741,519 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="C16">
         <v>86000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17">
+        <v>99000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="1">
+        <v>108109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="1">
+        <v>108109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="1">
+        <v>108000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1">
+        <v>99000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="1">
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1">
+        <v>109000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="1">
+        <v>98000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="1">
+        <v>112000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="1">
+        <v>103000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1">
+        <v>108000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="1">
+        <v>108000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="1">
+        <v>104000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="1">
+        <v>111000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="1">
+        <v>103000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="1">
+        <v>107000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="1">
+        <v>112000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="1">
+        <v>107000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="1">
+        <v>112000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="1">
+        <v>105106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="1">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="1">
+        <v>101000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="1">
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="1">
+        <v>106000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="1">
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="1">
+        <v>108109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="1">
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="1">
+        <v>101000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="1">
+        <v>102000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="1">
+        <v>98000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="1">
+        <v>108000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="1">
+        <v>97000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="1">
+        <v>98000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" s="1">
+        <v>111000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="1">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="1">
+        <v>102000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="1">
+        <v>108000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="1">
+        <v>108000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="1">
+        <v>103104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="1">
+        <v>103104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="1">
+        <v>99000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="1">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="1">
+        <v>111000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" s="1">
+        <v>103000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C62" s="1">
+        <v>110000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add missing space in "Rönne å" in riverinfo.xlsx
</commit_message>
<xml_diff>
--- a/data-raw/riverinfo.xlsx
+++ b/data-raw/riverinfo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
   <si>
     <t>haronr</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>Rolfsån</t>
-  </si>
-  <si>
-    <t>Rönneå</t>
   </si>
   <si>
     <t>Rördalsån</t>
@@ -566,7 +563,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -741,10 +740,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16">
         <v>86000</v>
@@ -755,7 +754,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17">
         <v>99000</v>
@@ -766,7 +765,7 @@
         <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1">
         <v>108109</v>
@@ -777,7 +776,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1">
         <v>108109</v>
@@ -788,7 +787,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1">
         <v>108000</v>
@@ -799,7 +798,7 @@
         <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1">
         <v>99000</v>
@@ -807,10 +806,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1">
         <v>96000</v>
@@ -832,7 +831,7 @@
         <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="1">
         <v>98000</v>
@@ -854,7 +853,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1">
         <v>103000</v>
@@ -865,7 +864,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1">
         <v>108000</v>
@@ -887,7 +886,7 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="1">
         <v>108000</v>
@@ -920,7 +919,7 @@
         <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="1">
         <v>103000</v>
@@ -939,7 +938,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>44</v>
@@ -975,7 +974,7 @@
         <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="1">
         <v>105106</v>
@@ -1008,7 +1007,7 @@
         <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1">
         <v>96000</v>
@@ -1027,10 +1026,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C42" s="1">
         <v>96000</v>
@@ -1038,10 +1037,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="1">
         <v>108109</v>
@@ -1049,10 +1048,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" s="1">
         <v>96000</v>
@@ -1071,7 +1070,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>33</v>
@@ -1085,7 +1084,7 @@
         <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="1">
         <v>98000</v>
@@ -1093,10 +1092,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" s="1">
         <v>108000</v>
@@ -1104,10 +1103,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" s="1">
         <v>97000</v>
@@ -1118,7 +1117,7 @@
         <v>30</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="1">
         <v>98000</v>
@@ -1162,7 +1161,7 @@
         <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" s="1">
         <v>108000</v>
@@ -1170,10 +1169,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55" s="1">
         <v>108000</v>
@@ -1184,7 +1183,7 @@
         <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" s="1">
         <v>103104</v>
@@ -1195,7 +1194,7 @@
         <v>36</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C57" s="1">
         <v>103104</v>
@@ -1206,7 +1205,7 @@
         <v>37</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1">
         <v>99000</v>
@@ -1225,7 +1224,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>31</v>
@@ -1236,10 +1235,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C61" s="1">
         <v>103000</v>

</xml_diff>